<commit_message>
Ajout de nouveaux animaux
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/ListeAnimaux.xlsx
+++ b/Fichiers modifiables/ListeAnimaux.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="573">
   <si>
     <t>name</t>
   </si>
@@ -1176,9 +1176,6 @@
     <t>2017-03-09</t>
   </si>
   <si>
-    <t>Y-m-d h:m</t>
-  </si>
-  <si>
     <t>2021-01-21 15:59:00</t>
   </si>
   <si>
@@ -1453,6 +1450,294 @@
   </si>
   <si>
     <t>2021-01-21 11:12:00</t>
+  </si>
+  <si>
+    <t>2020-05-16</t>
+  </si>
+  <si>
+    <t>Fuller</t>
+  </si>
+  <si>
+    <t>2020-04-03</t>
+  </si>
+  <si>
+    <t>Dexter</t>
+  </si>
+  <si>
+    <t>2021-01-15</t>
+  </si>
+  <si>
+    <t>Rudyard</t>
+  </si>
+  <si>
+    <t>2020-12-07</t>
+  </si>
+  <si>
+    <t>Chadwick</t>
+  </si>
+  <si>
+    <t>2020-10-30</t>
+  </si>
+  <si>
+    <t>Aladdin</t>
+  </si>
+  <si>
+    <t>2020-07-14</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>Bert</t>
+  </si>
+  <si>
+    <t>2020-06-09</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>2020-05-08</t>
+  </si>
+  <si>
+    <t>Erasmus</t>
+  </si>
+  <si>
+    <t>2020-11-24</t>
+  </si>
+  <si>
+    <t>Nichole</t>
+  </si>
+  <si>
+    <t>2020-12-03</t>
+  </si>
+  <si>
+    <t>2020-07-19</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>2020-02-26</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>2020-01-31</t>
+  </si>
+  <si>
+    <t>Darrel</t>
+  </si>
+  <si>
+    <t>2020-07-26</t>
+  </si>
+  <si>
+    <t>Giacomo</t>
+  </si>
+  <si>
+    <t>2020-08-12</t>
+  </si>
+  <si>
+    <t>Neil</t>
+  </si>
+  <si>
+    <t>2020-11-12</t>
+  </si>
+  <si>
+    <t>Chester</t>
+  </si>
+  <si>
+    <t>2020-10-21</t>
+  </si>
+  <si>
+    <t>Keane</t>
+  </si>
+  <si>
+    <t>2020-10-13</t>
+  </si>
+  <si>
+    <t>Clio</t>
+  </si>
+  <si>
+    <t>2020-07-18</t>
+  </si>
+  <si>
+    <t>2020-12-08</t>
+  </si>
+  <si>
+    <t>Orson</t>
+  </si>
+  <si>
+    <t>2020-08-19</t>
+  </si>
+  <si>
+    <t>Magee</t>
+  </si>
+  <si>
+    <t>2020-06-08</t>
+  </si>
+  <si>
+    <t>Kelsey</t>
+  </si>
+  <si>
+    <t>2020-06-10</t>
+  </si>
+  <si>
+    <t>Forrest</t>
+  </si>
+  <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>2020-01-06</t>
+  </si>
+  <si>
+    <t>2021-01-02</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>2020-09-17</t>
+  </si>
+  <si>
+    <t>Garrett</t>
+  </si>
+  <si>
+    <t>2020-03-15</t>
+  </si>
+  <si>
+    <t>Blair</t>
+  </si>
+  <si>
+    <t>2020-06-18</t>
+  </si>
+  <si>
+    <t>Malik</t>
+  </si>
+  <si>
+    <t>2020-03-19</t>
+  </si>
+  <si>
+    <t>2020-09-11</t>
+  </si>
+  <si>
+    <t>Lucian</t>
+  </si>
+  <si>
+    <t>2020-03-22</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>2020-01-29</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>2020-06-05</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>2020-05-12</t>
+  </si>
+  <si>
+    <t>Mufutau</t>
+  </si>
+  <si>
+    <t>2020-09-18</t>
+  </si>
+  <si>
+    <t>2020-09-27</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>2020-02-13</t>
+  </si>
+  <si>
+    <t>Quamar</t>
+  </si>
+  <si>
+    <t>2020-03-07</t>
+  </si>
+  <si>
+    <t>Marny</t>
+  </si>
+  <si>
+    <t>2020-02-12</t>
+  </si>
+  <si>
+    <t>Molly</t>
+  </si>
+  <si>
+    <t>2020-02-07</t>
+  </si>
+  <si>
+    <t>Emery</t>
+  </si>
+  <si>
+    <t>Declan</t>
+  </si>
+  <si>
+    <t>2020-03-10</t>
+  </si>
+  <si>
+    <t>Kevyn</t>
+  </si>
+  <si>
+    <t>2020-06-21</t>
+  </si>
+  <si>
+    <t>Brock</t>
+  </si>
+  <si>
+    <t>2020-06-13</t>
+  </si>
+  <si>
+    <t>Alden</t>
+  </si>
+  <si>
+    <t>2020-03-01</t>
+  </si>
+  <si>
+    <t>2020-11-09</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>2020-11-10</t>
+  </si>
+  <si>
+    <t>Fredericka</t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>Colin</t>
+  </si>
+  <si>
+    <t>2020-11-14</t>
+  </si>
+  <si>
+    <t>2020-03-17</t>
   </si>
 </sst>
 </file>
@@ -1813,10 +2098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L206"/>
+  <dimension ref="A1:L260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +2177,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1913,7 +2198,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1934,7 +2219,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1961,7 +2246,7 @@
         <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1982,7 +2267,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2009,7 +2294,7 @@
         <v>14</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2030,7 +2315,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2057,7 +2342,7 @@
         <v>14</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2078,7 +2363,7 @@
       </c>
       <c r="F11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2105,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2132,7 +2417,7 @@
         <v>5</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2152,7 +2437,7 @@
         <v>2</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2171,11 +2456,12 @@
       <c r="E15">
         <v>2</v>
       </c>
+      <c r="F15" s="1"/>
       <c r="H15">
         <v>28</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2195,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,7 +2504,7 @@
         <v>57</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2238,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2264,7 +2550,7 @@
         <v>73</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2284,14 +2570,14 @@
         <v>1</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2304,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2324,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2347,7 +2633,7 @@
         <v>27</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2370,7 +2656,7 @@
         <v>27</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2393,7 +2679,7 @@
         <v>27</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2413,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2436,7 +2722,7 @@
         <v>27</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2456,7 +2742,7 @@
         <v>2</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2482,7 +2768,7 @@
         <v>27</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2502,7 +2788,7 @@
         <v>2</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2522,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,7 +2828,7 @@
         <v>2</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2561,8 +2847,9 @@
       <c r="E33">
         <v>1</v>
       </c>
+      <c r="F33" s="1"/>
       <c r="L33" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2588,7 +2875,7 @@
         <v>198</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2614,7 +2901,7 @@
         <v>198</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2640,7 +2927,7 @@
         <v>198</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2659,8 +2946,9 @@
       <c r="E37">
         <v>1</v>
       </c>
+      <c r="F37" s="1"/>
       <c r="L37" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2680,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2700,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2720,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2740,7 +3028,7 @@
         <v>2</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2760,7 +3048,7 @@
         <v>2</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2780,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2803,7 +3091,7 @@
         <v>38</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2826,7 +3114,7 @@
         <v>38</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2846,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2872,7 +3160,7 @@
         <v>129</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2892,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2912,7 +3200,7 @@
         <v>2</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2932,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2958,7 +3246,7 @@
         <v>25</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2984,7 +3272,7 @@
         <v>25</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3004,7 +3292,7 @@
         <v>2</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3024,7 +3312,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3050,7 +3338,7 @@
         <v>81</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3076,7 +3364,7 @@
         <v>81</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3102,7 +3390,7 @@
         <v>140</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3122,7 +3410,7 @@
         <v>2</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3142,7 +3430,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3161,14 +3449,14 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="1">
         <v>13</v>
       </c>
       <c r="I60">
         <v>24</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3194,7 +3482,7 @@
         <v>24</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3214,7 +3502,7 @@
         <v>2</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3237,7 +3525,7 @@
         <v>77</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3260,7 +3548,7 @@
         <v>84</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3279,8 +3567,9 @@
       <c r="E65">
         <v>1</v>
       </c>
+      <c r="F65" s="1"/>
       <c r="L65" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3303,7 +3592,7 @@
         <v>45</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3323,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3346,7 +3635,7 @@
         <v>97</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3366,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3386,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3407,7 +3696,7 @@
       </c>
       <c r="H71" s="3"/>
       <c r="L71" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3433,7 +3722,7 @@
         <v>16</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3459,7 +3748,7 @@
         <v>16</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3479,7 +3768,7 @@
         <v>2</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3499,7 +3788,7 @@
         <v>2</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3522,7 +3811,7 @@
         <v>10</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3545,7 +3834,7 @@
         <v>10</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3568,7 +3857,7 @@
         <v>89</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3591,78 +3880,78 @@
         <v>51</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="80" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D80" s="1">
         <v>11</v>
       </c>
       <c r="E80" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>37</v>
+        <v>341</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>376</v>
       </c>
       <c r="D81">
         <v>11</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>202</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>378</v>
+        <v>8</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D82" s="1">
         <v>12</v>
       </c>
       <c r="E82" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="D83">
         <v>12</v>
@@ -3670,19 +3959,25 @@
       <c r="E83">
         <v>2</v>
       </c>
+      <c r="H83">
+        <v>8</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
       <c r="L83" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="D84">
         <v>12</v>
@@ -3690,6 +3985,7 @@
       <c r="E84">
         <v>2</v>
       </c>
+      <c r="F84" s="1"/>
       <c r="H84">
         <v>8</v>
       </c>
@@ -3697,33 +3993,27 @@
         <v>1</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>181</v>
-      </c>
-      <c r="B85" t="s">
-        <v>183</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>184</v>
+        <v>202</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>378</v>
       </c>
       <c r="D85">
         <v>12</v>
       </c>
       <c r="E85">
-        <v>2</v>
-      </c>
-      <c r="H85">
-        <v>8</v>
-      </c>
-      <c r="I85">
         <v>1</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3743,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -3763,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -3783,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -3803,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -3823,7 +4113,7 @@
         <v>2</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -3843,7 +4133,7 @@
         <v>2</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -3869,7 +4159,7 @@
         <v>114</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -3889,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -3909,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -3929,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -3955,7 +4245,7 @@
         <v>12</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -3978,7 +4268,7 @@
         <v>33</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -3998,7 +4288,7 @@
         <v>2</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -4024,7 +4314,7 @@
         <v>12</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4044,7 +4334,7 @@
         <v>2</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -4064,7 +4354,7 @@
         <v>2</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -4087,7 +4377,7 @@
         <v>42</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -4260,6 +4550,7 @@
       <c r="E111" s="1">
         <v>2</v>
       </c>
+      <c r="F111" s="1"/>
       <c r="I111">
         <v>46</v>
       </c>
@@ -4322,6 +4613,9 @@
       </c>
     </row>
     <row r="115" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>203</v>
+      </c>
       <c r="B115" s="1" t="s">
         <v>310</v>
       </c>
@@ -4392,6 +4686,7 @@
       <c r="E118" s="1">
         <v>2</v>
       </c>
+      <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -4558,6 +4853,7 @@
       <c r="E126" s="1">
         <v>1</v>
       </c>
+      <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
@@ -4575,6 +4871,7 @@
       <c r="E127" s="1">
         <v>1</v>
       </c>
+      <c r="F127" s="1"/>
       <c r="H127">
         <v>85</v>
       </c>
@@ -4655,6 +4952,7 @@
       <c r="E131" s="1">
         <v>2</v>
       </c>
+      <c r="F131" s="1"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
@@ -4743,38 +5041,44 @@
       </c>
     </row>
     <row r="136" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>187</v>
+      </c>
       <c r="B136" s="1" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D136" s="1">
         <v>22</v>
       </c>
       <c r="E136" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L136" s="2"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D137" s="1">
         <v>22</v>
       </c>
       <c r="E137" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>205</v>
+      </c>
       <c r="B138" s="1" t="s">
         <v>382</v>
       </c>
@@ -4977,7 +5281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2</v>
       </c>
@@ -5491,6 +5795,7 @@
       <c r="E176" s="1">
         <v>1</v>
       </c>
+      <c r="F176" s="1"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
@@ -5685,7 +5990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>11</v>
       </c>
@@ -6068,9 +6373,927 @@
         <v>50</v>
       </c>
     </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>208</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D207" s="1">
+        <v>40</v>
+      </c>
+      <c r="E207" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>210</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D208" s="1">
+        <v>40</v>
+      </c>
+      <c r="E208" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>212</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D209" s="1">
+        <v>40</v>
+      </c>
+      <c r="E209" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>218</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D210" s="1">
+        <v>40</v>
+      </c>
+      <c r="E210" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>231</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D211" s="1">
+        <v>40</v>
+      </c>
+      <c r="E211" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>247</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D212" s="1">
+        <v>40</v>
+      </c>
+      <c r="E212" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>254</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D213" s="1">
+        <v>40</v>
+      </c>
+      <c r="E213" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>214</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D214" s="1">
+        <v>41</v>
+      </c>
+      <c r="E214" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>221</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D215" s="1">
+        <v>41</v>
+      </c>
+      <c r="E215" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>230</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D216" s="1">
+        <v>41</v>
+      </c>
+      <c r="E216" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>245</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D217" s="1">
+        <v>41</v>
+      </c>
+      <c r="E217" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>206</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D218" s="1">
+        <v>42</v>
+      </c>
+      <c r="E218" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>248</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D219" s="1">
+        <v>42</v>
+      </c>
+      <c r="E219" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>253</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="D220" s="1">
+        <v>42</v>
+      </c>
+      <c r="E220" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>207</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D221" s="1">
+        <v>43</v>
+      </c>
+      <c r="E221" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>234</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D222" s="1">
+        <v>43</v>
+      </c>
+      <c r="E222" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>238</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D223" s="1">
+        <v>43</v>
+      </c>
+      <c r="E223" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>240</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D224" s="1">
+        <v>43</v>
+      </c>
+      <c r="E224" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>255</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D225" s="1">
+        <v>43</v>
+      </c>
+      <c r="E225" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>211</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D226" s="1">
+        <v>44</v>
+      </c>
+      <c r="E226" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>228</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D227" s="1">
+        <v>44</v>
+      </c>
+      <c r="E227" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>235</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D228" s="1">
+        <v>44</v>
+      </c>
+      <c r="E228" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>236</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D229" s="1">
+        <v>44</v>
+      </c>
+      <c r="E229" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>229</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D230" s="1">
+        <v>45</v>
+      </c>
+      <c r="E230" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>241</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D231" s="1">
+        <v>45</v>
+      </c>
+      <c r="E231" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>251</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D232" s="1">
+        <v>45</v>
+      </c>
+      <c r="E232" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>252</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D233" s="1">
+        <v>45</v>
+      </c>
+      <c r="E233" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>258</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="D234" s="1">
+        <v>45</v>
+      </c>
+      <c r="E234" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>209</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D235" s="1">
+        <v>46</v>
+      </c>
+      <c r="E235" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>223</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D236" s="1">
+        <v>46</v>
+      </c>
+      <c r="E236" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>225</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D237" s="1">
+        <v>46</v>
+      </c>
+      <c r="E237" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>232</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D238" s="1">
+        <v>46</v>
+      </c>
+      <c r="E238" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>237</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D239" s="1">
+        <v>46</v>
+      </c>
+      <c r="E239" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>239</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D240" s="1">
+        <v>46</v>
+      </c>
+      <c r="E240" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>243</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D241" s="1">
+        <v>46</v>
+      </c>
+      <c r="E241" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>219</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D242" s="1">
+        <v>47</v>
+      </c>
+      <c r="E242" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>222</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D243" s="1">
+        <v>47</v>
+      </c>
+      <c r="E243" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>244</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D244" s="1">
+        <v>47</v>
+      </c>
+      <c r="E244" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>256</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D245" s="1">
+        <v>47</v>
+      </c>
+      <c r="E245" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>257</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="D246" s="1">
+        <v>47</v>
+      </c>
+      <c r="E246" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>213</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D247" s="1">
+        <v>48</v>
+      </c>
+      <c r="E247" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>215</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D248" s="1">
+        <v>48</v>
+      </c>
+      <c r="E248" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>216</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D249" s="1">
+        <v>48</v>
+      </c>
+      <c r="E249" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>220</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D250" s="1">
+        <v>48</v>
+      </c>
+      <c r="E250" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>226</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D251" s="1">
+        <v>48</v>
+      </c>
+      <c r="E251" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>227</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D252" s="1">
+        <v>48</v>
+      </c>
+      <c r="E252" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>233</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D253" s="1">
+        <v>48</v>
+      </c>
+      <c r="E253" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>242</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D254" s="1">
+        <v>48</v>
+      </c>
+      <c r="E254" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>250</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D255" s="1">
+        <v>48</v>
+      </c>
+      <c r="E255" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>259</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D256" s="1">
+        <v>48</v>
+      </c>
+      <c r="E256" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>217</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D257" s="1">
+        <v>49</v>
+      </c>
+      <c r="E257" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>224</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D258" s="1">
+        <v>49</v>
+      </c>
+      <c r="E258" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>246</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D259" s="1">
+        <v>49</v>
+      </c>
+      <c r="E259" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>249</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D260" s="1">
+        <v>49</v>
+      </c>
+      <c r="E260" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState ref="A2:I201">
+  <sortState ref="A2:I260">
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">

</xml_diff>

<commit_message>
ajout des enclos, types, secteurs
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/ListeAnimaux.xlsx
+++ b/Fichiers modifiables/ListeAnimaux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\Fichiers modifiables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paola.costa\Documents\GitHub\Ma-08_Zoo\Fichiers modifiables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2100,15 +2100,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="I258" sqref="I258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2158,6 +2158,9 @@
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
+      <c r="G2">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2176,6 +2179,9 @@
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
+      <c r="G3" s="1">
+        <v>27</v>
+      </c>
       <c r="L3" s="2" t="s">
         <v>385</v>
       </c>
@@ -2197,6 +2203,9 @@
         <v>2</v>
       </c>
       <c r="F4" s="2"/>
+      <c r="G4" s="1">
+        <v>27</v>
+      </c>
       <c r="L4" s="2" t="s">
         <v>386</v>
       </c>
@@ -2218,6 +2227,9 @@
         <v>2</v>
       </c>
       <c r="F5" s="2"/>
+      <c r="G5" s="1">
+        <v>27</v>
+      </c>
       <c r="L5" s="2" t="s">
         <v>387</v>
       </c>
@@ -2239,6 +2251,9 @@
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <v>27</v>
+      </c>
       <c r="H6" s="1">
         <v>32</v>
       </c>
@@ -2266,6 +2281,9 @@
         <v>1</v>
       </c>
       <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <v>27</v>
+      </c>
       <c r="L7" s="2" t="s">
         <v>389</v>
       </c>
@@ -2287,6 +2305,9 @@
         <v>1</v>
       </c>
       <c r="F8" s="2"/>
+      <c r="G8" s="1">
+        <v>27</v>
+      </c>
       <c r="H8" s="1">
         <v>32</v>
       </c>
@@ -2314,6 +2335,9 @@
         <v>2</v>
       </c>
       <c r="F9" s="2"/>
+      <c r="G9" s="1">
+        <v>27</v>
+      </c>
       <c r="L9" s="2" t="s">
         <v>391</v>
       </c>
@@ -2335,6 +2359,9 @@
         <v>1</v>
       </c>
       <c r="F10" s="2"/>
+      <c r="G10" s="1">
+        <v>27</v>
+      </c>
       <c r="H10">
         <v>32</v>
       </c>
@@ -2362,6 +2389,9 @@
         <v>1</v>
       </c>
       <c r="F11" s="2"/>
+      <c r="G11" s="1">
+        <v>27</v>
+      </c>
       <c r="L11" s="2" t="s">
         <v>393</v>
       </c>
@@ -2383,6 +2413,9 @@
         <v>2</v>
       </c>
       <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <v>27</v>
+      </c>
       <c r="H12">
         <v>36</v>
       </c>
@@ -2410,6 +2443,9 @@
         <v>2</v>
       </c>
       <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <v>27</v>
+      </c>
       <c r="H13">
         <v>32</v>
       </c>
@@ -2436,6 +2472,9 @@
       <c r="E14">
         <v>2</v>
       </c>
+      <c r="G14">
+        <v>55</v>
+      </c>
       <c r="L14" s="2" t="s">
         <v>396</v>
       </c>
@@ -2457,6 +2496,9 @@
         <v>2</v>
       </c>
       <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>55</v>
+      </c>
       <c r="H15">
         <v>28</v>
       </c>
@@ -2480,6 +2522,9 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="G16" s="1">
+        <v>55</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>398</v>
       </c>
@@ -2500,6 +2545,9 @@
       <c r="E17">
         <v>1</v>
       </c>
+      <c r="G17" s="1">
+        <v>55</v>
+      </c>
       <c r="H17">
         <v>57</v>
       </c>
@@ -2523,6 +2571,9 @@
       <c r="E18">
         <v>2</v>
       </c>
+      <c r="G18" s="1">
+        <v>55</v>
+      </c>
       <c r="L18" s="2" t="s">
         <v>400</v>
       </c>
@@ -2543,6 +2594,9 @@
       <c r="E19">
         <v>2</v>
       </c>
+      <c r="G19" s="1">
+        <v>55</v>
+      </c>
       <c r="H19">
         <v>28</v>
       </c>
@@ -2569,6 +2623,9 @@
       <c r="E20">
         <v>1</v>
       </c>
+      <c r="G20">
+        <v>49</v>
+      </c>
       <c r="L20" s="2" t="s">
         <v>402</v>
       </c>
@@ -2589,6 +2646,9 @@
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="G21" s="1">
+        <v>49</v>
+      </c>
       <c r="L21" s="2" t="s">
         <v>403</v>
       </c>
@@ -2609,6 +2669,9 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="G22" s="1">
+        <v>49</v>
+      </c>
       <c r="L22" s="2" t="s">
         <v>404</v>
       </c>
@@ -2629,6 +2692,9 @@
       <c r="E23">
         <v>1</v>
       </c>
+      <c r="G23" s="1">
+        <v>49</v>
+      </c>
       <c r="I23">
         <v>27</v>
       </c>
@@ -2652,6 +2718,9 @@
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="G24" s="1">
+        <v>49</v>
+      </c>
       <c r="I24">
         <v>27</v>
       </c>
@@ -2675,6 +2744,9 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="G25" s="1">
+        <v>49</v>
+      </c>
       <c r="I25">
         <v>27</v>
       </c>
@@ -2698,6 +2770,9 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="G26" s="1">
+        <v>49</v>
+      </c>
       <c r="L26" s="2" t="s">
         <v>405</v>
       </c>
@@ -2718,6 +2793,9 @@
       <c r="E27">
         <v>2</v>
       </c>
+      <c r="G27" s="1">
+        <v>49</v>
+      </c>
       <c r="I27">
         <v>27</v>
       </c>
@@ -2741,6 +2819,9 @@
       <c r="E28">
         <v>2</v>
       </c>
+      <c r="G28" s="1">
+        <v>49</v>
+      </c>
       <c r="L28" s="2" t="s">
         <v>409</v>
       </c>
@@ -2761,6 +2842,9 @@
       <c r="E29">
         <v>1</v>
       </c>
+      <c r="G29" s="1">
+        <v>49</v>
+      </c>
       <c r="H29">
         <v>179</v>
       </c>
@@ -2787,6 +2871,9 @@
       <c r="E30">
         <v>2</v>
       </c>
+      <c r="G30">
+        <v>54</v>
+      </c>
       <c r="L30" s="2" t="s">
         <v>411</v>
       </c>
@@ -2807,6 +2894,9 @@
       <c r="E31">
         <v>2</v>
       </c>
+      <c r="G31">
+        <v>54</v>
+      </c>
       <c r="L31" s="2" t="s">
         <v>412</v>
       </c>
@@ -2827,6 +2917,9 @@
       <c r="E32">
         <v>2</v>
       </c>
+      <c r="G32">
+        <v>54</v>
+      </c>
       <c r="L32" s="2" t="s">
         <v>413</v>
       </c>
@@ -2848,6 +2941,9 @@
         <v>1</v>
       </c>
       <c r="F33" s="1"/>
+      <c r="G33">
+        <v>54</v>
+      </c>
       <c r="L33" s="2" t="s">
         <v>414</v>
       </c>
@@ -2868,6 +2964,9 @@
       <c r="E34">
         <v>2</v>
       </c>
+      <c r="G34">
+        <v>54</v>
+      </c>
       <c r="H34">
         <v>58</v>
       </c>
@@ -2894,6 +2993,9 @@
       <c r="E35">
         <v>1</v>
       </c>
+      <c r="G35">
+        <v>54</v>
+      </c>
       <c r="H35">
         <v>58</v>
       </c>
@@ -2920,6 +3022,9 @@
       <c r="E36">
         <v>2</v>
       </c>
+      <c r="G36">
+        <v>54</v>
+      </c>
       <c r="H36" s="1">
         <v>69</v>
       </c>
@@ -2947,6 +3052,9 @@
         <v>1</v>
       </c>
       <c r="F37" s="1"/>
+      <c r="G37">
+        <v>61</v>
+      </c>
       <c r="L37" s="2" t="s">
         <v>418</v>
       </c>
@@ -2967,6 +3075,9 @@
       <c r="E38">
         <v>1</v>
       </c>
+      <c r="G38">
+        <v>61</v>
+      </c>
       <c r="L38" s="2" t="s">
         <v>419</v>
       </c>
@@ -2987,6 +3098,9 @@
       <c r="E39">
         <v>1</v>
       </c>
+      <c r="G39">
+        <v>61</v>
+      </c>
       <c r="L39" s="2" t="s">
         <v>401</v>
       </c>
@@ -3007,6 +3121,9 @@
       <c r="E40">
         <v>1</v>
       </c>
+      <c r="G40">
+        <v>61</v>
+      </c>
       <c r="L40" s="2" t="s">
         <v>420</v>
       </c>
@@ -3027,6 +3144,9 @@
       <c r="E41">
         <v>2</v>
       </c>
+      <c r="G41">
+        <v>61</v>
+      </c>
       <c r="L41" s="2" t="s">
         <v>421</v>
       </c>
@@ -3047,6 +3167,9 @@
       <c r="E42">
         <v>2</v>
       </c>
+      <c r="G42">
+        <v>61</v>
+      </c>
       <c r="L42" s="2" t="s">
         <v>422</v>
       </c>
@@ -3067,6 +3190,9 @@
       <c r="E43">
         <v>1</v>
       </c>
+      <c r="G43">
+        <v>61</v>
+      </c>
       <c r="L43" s="2" t="s">
         <v>423</v>
       </c>
@@ -3087,6 +3213,9 @@
       <c r="E44">
         <v>2</v>
       </c>
+      <c r="G44" s="1">
+        <v>61</v>
+      </c>
       <c r="H44">
         <v>38</v>
       </c>
@@ -3110,6 +3239,9 @@
       <c r="E45">
         <v>1</v>
       </c>
+      <c r="G45" s="1">
+        <v>61</v>
+      </c>
       <c r="H45">
         <v>38</v>
       </c>
@@ -3133,6 +3265,9 @@
       <c r="E46">
         <v>2</v>
       </c>
+      <c r="G46" s="1">
+        <v>61</v>
+      </c>
       <c r="L46" s="2" t="s">
         <v>426</v>
       </c>
@@ -3153,6 +3288,9 @@
       <c r="E47">
         <v>2</v>
       </c>
+      <c r="G47" s="1">
+        <v>61</v>
+      </c>
       <c r="H47">
         <v>83</v>
       </c>
@@ -3179,6 +3317,9 @@
       <c r="E48">
         <v>1</v>
       </c>
+      <c r="G48">
+        <v>59</v>
+      </c>
       <c r="L48" s="2" t="s">
         <v>428</v>
       </c>
@@ -3199,6 +3340,9 @@
       <c r="E49">
         <v>2</v>
       </c>
+      <c r="G49" s="1">
+        <v>59</v>
+      </c>
       <c r="L49" s="2" t="s">
         <v>429</v>
       </c>
@@ -3219,6 +3363,9 @@
       <c r="E50">
         <v>2</v>
       </c>
+      <c r="G50" s="1">
+        <v>59</v>
+      </c>
       <c r="L50" s="2" t="s">
         <v>430</v>
       </c>
@@ -3239,6 +3386,9 @@
       <c r="E51">
         <v>1</v>
       </c>
+      <c r="G51" s="1">
+        <v>59</v>
+      </c>
       <c r="H51">
         <v>29</v>
       </c>
@@ -3265,6 +3415,9 @@
       <c r="E52">
         <v>2</v>
       </c>
+      <c r="G52" s="1">
+        <v>59</v>
+      </c>
       <c r="H52">
         <v>34</v>
       </c>
@@ -3291,6 +3444,9 @@
       <c r="E53">
         <v>2</v>
       </c>
+      <c r="G53" s="1">
+        <v>59</v>
+      </c>
       <c r="L53" s="2" t="s">
         <v>433</v>
       </c>
@@ -3311,6 +3467,9 @@
       <c r="E54">
         <v>1</v>
       </c>
+      <c r="G54" s="1">
+        <v>59</v>
+      </c>
       <c r="L54" s="2" t="s">
         <v>434</v>
       </c>
@@ -3331,6 +3490,9 @@
       <c r="E55">
         <v>1</v>
       </c>
+      <c r="G55" s="1">
+        <v>59</v>
+      </c>
       <c r="H55">
         <v>122</v>
       </c>
@@ -3357,6 +3519,9 @@
       <c r="E56">
         <v>2</v>
       </c>
+      <c r="G56" s="1">
+        <v>59</v>
+      </c>
       <c r="H56">
         <v>122</v>
       </c>
@@ -3383,6 +3548,9 @@
       <c r="E57">
         <v>2</v>
       </c>
+      <c r="G57" s="1">
+        <v>59</v>
+      </c>
       <c r="H57">
         <v>158</v>
       </c>
@@ -3409,6 +3577,9 @@
       <c r="E58">
         <v>2</v>
       </c>
+      <c r="G58">
+        <v>93</v>
+      </c>
       <c r="L58" s="2" t="s">
         <v>438</v>
       </c>
@@ -3429,6 +3600,9 @@
       <c r="E59">
         <v>1</v>
       </c>
+      <c r="G59" s="1">
+        <v>93</v>
+      </c>
       <c r="L59" s="2" t="s">
         <v>439</v>
       </c>
@@ -3449,6 +3623,9 @@
       <c r="E60">
         <v>1</v>
       </c>
+      <c r="G60" s="1">
+        <v>93</v>
+      </c>
       <c r="H60" s="1">
         <v>13</v>
       </c>
@@ -3475,6 +3652,9 @@
       <c r="E61">
         <v>1</v>
       </c>
+      <c r="G61" s="1">
+        <v>93</v>
+      </c>
       <c r="H61">
         <v>13</v>
       </c>
@@ -3501,6 +3681,9 @@
       <c r="E62">
         <v>2</v>
       </c>
+      <c r="G62" s="1">
+        <v>93</v>
+      </c>
       <c r="L62" s="2" t="s">
         <v>442</v>
       </c>
@@ -3521,6 +3704,9 @@
       <c r="E63">
         <v>2</v>
       </c>
+      <c r="G63" s="1">
+        <v>93</v>
+      </c>
       <c r="I63">
         <v>77</v>
       </c>
@@ -3544,6 +3730,9 @@
       <c r="E64">
         <v>2</v>
       </c>
+      <c r="G64" s="1">
+        <v>93</v>
+      </c>
       <c r="H64">
         <v>84</v>
       </c>
@@ -3568,6 +3757,9 @@
         <v>1</v>
       </c>
       <c r="F65" s="1"/>
+      <c r="G65">
+        <v>86</v>
+      </c>
       <c r="L65" s="2" t="s">
         <v>445</v>
       </c>
@@ -3588,6 +3780,9 @@
       <c r="E66">
         <v>1</v>
       </c>
+      <c r="G66" s="1">
+        <v>86</v>
+      </c>
       <c r="I66">
         <v>45</v>
       </c>
@@ -3611,6 +3806,9 @@
       <c r="E67">
         <v>1</v>
       </c>
+      <c r="G67" s="1">
+        <v>86</v>
+      </c>
       <c r="L67" s="2" t="s">
         <v>444</v>
       </c>
@@ -3631,6 +3829,9 @@
       <c r="E68">
         <v>2</v>
       </c>
+      <c r="G68" s="1">
+        <v>86</v>
+      </c>
       <c r="I68">
         <v>97</v>
       </c>
@@ -3654,6 +3855,9 @@
       <c r="E69">
         <v>1</v>
       </c>
+      <c r="G69" s="1">
+        <v>69</v>
+      </c>
       <c r="L69" s="2" t="s">
         <v>448</v>
       </c>
@@ -3674,6 +3878,9 @@
       <c r="E70">
         <v>1</v>
       </c>
+      <c r="G70" s="1">
+        <v>69</v>
+      </c>
       <c r="L70" s="2" t="s">
         <v>449</v>
       </c>
@@ -3694,6 +3901,9 @@
       <c r="E71">
         <v>2</v>
       </c>
+      <c r="G71" s="1">
+        <v>69</v>
+      </c>
       <c r="H71" s="3"/>
       <c r="L71" s="2" t="s">
         <v>450</v>
@@ -3715,6 +3925,9 @@
       <c r="E72">
         <v>2</v>
       </c>
+      <c r="G72" s="1">
+        <v>69</v>
+      </c>
       <c r="H72">
         <v>59</v>
       </c>
@@ -3741,6 +3954,9 @@
       <c r="E73">
         <v>2</v>
       </c>
+      <c r="G73" s="1">
+        <v>69</v>
+      </c>
       <c r="H73">
         <v>59</v>
       </c>
@@ -3767,6 +3983,9 @@
       <c r="E74">
         <v>2</v>
       </c>
+      <c r="G74">
+        <v>72</v>
+      </c>
       <c r="L74" s="2" t="s">
         <v>453</v>
       </c>
@@ -3787,6 +4006,9 @@
       <c r="E75">
         <v>2</v>
       </c>
+      <c r="G75" s="1">
+        <v>72</v>
+      </c>
       <c r="L75" s="2" t="s">
         <v>454</v>
       </c>
@@ -3807,6 +4029,9 @@
       <c r="E76">
         <v>2</v>
       </c>
+      <c r="G76" s="1">
+        <v>72</v>
+      </c>
       <c r="H76">
         <v>10</v>
       </c>
@@ -3830,6 +4055,9 @@
       <c r="E77">
         <v>2</v>
       </c>
+      <c r="G77" s="1">
+        <v>72</v>
+      </c>
       <c r="H77">
         <v>10</v>
       </c>
@@ -3853,6 +4081,9 @@
       <c r="E78">
         <v>1</v>
       </c>
+      <c r="G78" s="1">
+        <v>72</v>
+      </c>
       <c r="H78">
         <v>89</v>
       </c>
@@ -3876,6 +4107,9 @@
       <c r="E79">
         <v>1</v>
       </c>
+      <c r="G79" s="1">
+        <v>72</v>
+      </c>
       <c r="H79">
         <v>51</v>
       </c>
@@ -3899,6 +4133,9 @@
       <c r="E80" s="1">
         <v>2</v>
       </c>
+      <c r="G80" s="1">
+        <v>71</v>
+      </c>
       <c r="L80" s="2" t="s">
         <v>421</v>
       </c>
@@ -3919,6 +4156,9 @@
       <c r="E81">
         <v>1</v>
       </c>
+      <c r="G81" s="1">
+        <v>71</v>
+      </c>
       <c r="L81" s="2" t="s">
         <v>459</v>
       </c>
@@ -3939,6 +4179,9 @@
       <c r="E82" s="1">
         <v>2</v>
       </c>
+      <c r="G82" s="1">
+        <v>52</v>
+      </c>
       <c r="L82" s="2" t="s">
         <v>460</v>
       </c>
@@ -3959,6 +4202,9 @@
       <c r="E83">
         <v>2</v>
       </c>
+      <c r="G83" s="1">
+        <v>52</v>
+      </c>
       <c r="H83">
         <v>8</v>
       </c>
@@ -3986,6 +4232,9 @@
         <v>2</v>
       </c>
       <c r="F84" s="1"/>
+      <c r="G84" s="1">
+        <v>52</v>
+      </c>
       <c r="H84">
         <v>8</v>
       </c>
@@ -4012,6 +4261,9 @@
       <c r="E85">
         <v>1</v>
       </c>
+      <c r="G85" s="1">
+        <v>52</v>
+      </c>
       <c r="L85" s="2" t="s">
         <v>463</v>
       </c>
@@ -4032,6 +4284,9 @@
       <c r="E86">
         <v>2</v>
       </c>
+      <c r="G86">
+        <v>95</v>
+      </c>
       <c r="L86" s="2" t="s">
         <v>433</v>
       </c>
@@ -4052,6 +4307,9 @@
       <c r="E87">
         <v>1</v>
       </c>
+      <c r="G87" s="1">
+        <v>95</v>
+      </c>
       <c r="L87" s="2" t="s">
         <v>464</v>
       </c>
@@ -4072,6 +4330,9 @@
       <c r="E88">
         <v>2</v>
       </c>
+      <c r="G88" s="1">
+        <v>95</v>
+      </c>
       <c r="L88" s="2" t="s">
         <v>465</v>
       </c>
@@ -4092,6 +4353,9 @@
       <c r="E89">
         <v>1</v>
       </c>
+      <c r="G89" s="1">
+        <v>95</v>
+      </c>
       <c r="L89" s="2" t="s">
         <v>466</v>
       </c>
@@ -4112,6 +4376,9 @@
       <c r="E90">
         <v>2</v>
       </c>
+      <c r="G90" s="1">
+        <v>95</v>
+      </c>
       <c r="L90" s="2" t="s">
         <v>467</v>
       </c>
@@ -4132,6 +4399,9 @@
       <c r="E91">
         <v>2</v>
       </c>
+      <c r="G91" s="1">
+        <v>95</v>
+      </c>
       <c r="L91" s="2" t="s">
         <v>468</v>
       </c>
@@ -4152,6 +4422,9 @@
       <c r="E92">
         <v>1</v>
       </c>
+      <c r="G92" s="1">
+        <v>95</v>
+      </c>
       <c r="H92">
         <v>132</v>
       </c>
@@ -4178,6 +4451,9 @@
       <c r="E93">
         <v>1</v>
       </c>
+      <c r="G93">
+        <v>48</v>
+      </c>
       <c r="L93" s="2" t="s">
         <v>445</v>
       </c>
@@ -4198,6 +4474,9 @@
       <c r="E94">
         <v>2</v>
       </c>
+      <c r="G94" s="1">
+        <v>48</v>
+      </c>
       <c r="L94" s="2" t="s">
         <v>470</v>
       </c>
@@ -4218,6 +4497,9 @@
       <c r="E95">
         <v>1</v>
       </c>
+      <c r="G95" s="1">
+        <v>48</v>
+      </c>
       <c r="L95" s="2" t="s">
         <v>471</v>
       </c>
@@ -4238,6 +4520,9 @@
       <c r="E96">
         <v>2</v>
       </c>
+      <c r="G96" s="1">
+        <v>48</v>
+      </c>
       <c r="H96">
         <v>14</v>
       </c>
@@ -4264,6 +4549,9 @@
       <c r="E97">
         <v>2</v>
       </c>
+      <c r="G97" s="1">
+        <v>48</v>
+      </c>
       <c r="I97">
         <v>33</v>
       </c>
@@ -4287,6 +4575,9 @@
       <c r="E98">
         <v>2</v>
       </c>
+      <c r="G98" s="1">
+        <v>48</v>
+      </c>
       <c r="L98" s="2" t="s">
         <v>474</v>
       </c>
@@ -4307,6 +4598,9 @@
       <c r="E99">
         <v>2</v>
       </c>
+      <c r="G99" s="1">
+        <v>48</v>
+      </c>
       <c r="H99">
         <v>14</v>
       </c>
@@ -4333,6 +4627,9 @@
       <c r="E100">
         <v>2</v>
       </c>
+      <c r="G100">
+        <v>88</v>
+      </c>
       <c r="L100" s="2" t="s">
         <v>449</v>
       </c>
@@ -4353,6 +4650,9 @@
       <c r="E101">
         <v>2</v>
       </c>
+      <c r="G101" s="1">
+        <v>88</v>
+      </c>
       <c r="L101" s="2" t="s">
         <v>476</v>
       </c>
@@ -4373,6 +4673,9 @@
       <c r="E102">
         <v>2</v>
       </c>
+      <c r="G102" s="1">
+        <v>88</v>
+      </c>
       <c r="H102">
         <v>42</v>
       </c>
@@ -4396,6 +4699,9 @@
       <c r="E103">
         <v>1</v>
       </c>
+      <c r="G103" s="1">
+        <v>88</v>
+      </c>
       <c r="H103">
         <v>48</v>
       </c>
@@ -4416,6 +4722,9 @@
       <c r="E104" s="1">
         <v>2</v>
       </c>
+      <c r="G104" s="1">
+        <v>88</v>
+      </c>
       <c r="H104">
         <v>48</v>
       </c>
@@ -4436,6 +4745,9 @@
       <c r="E105" s="1">
         <v>1</v>
       </c>
+      <c r="G105" s="1">
+        <v>88</v>
+      </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -4453,6 +4765,9 @@
       <c r="E106" s="1">
         <v>1</v>
       </c>
+      <c r="G106" s="1">
+        <v>88</v>
+      </c>
       <c r="H106">
         <v>62</v>
       </c>
@@ -4476,6 +4791,9 @@
       <c r="E107" s="1">
         <v>2</v>
       </c>
+      <c r="G107" s="1">
+        <v>88</v>
+      </c>
       <c r="H107">
         <v>62</v>
       </c>
@@ -4499,6 +4817,9 @@
       <c r="E108" s="1">
         <v>1</v>
       </c>
+      <c r="G108">
+        <v>25</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
@@ -4516,6 +4837,9 @@
       <c r="E109" s="1">
         <v>1</v>
       </c>
+      <c r="G109" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
@@ -4533,6 +4857,9 @@
       <c r="E110" s="1">
         <v>1</v>
       </c>
+      <c r="G110" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
@@ -4551,6 +4878,9 @@
         <v>2</v>
       </c>
       <c r="F111" s="1"/>
+      <c r="G111" s="1">
+        <v>25</v>
+      </c>
       <c r="I111">
         <v>46</v>
       </c>
@@ -4571,6 +4901,9 @@
       <c r="E112" s="1">
         <v>2</v>
       </c>
+      <c r="G112" s="1">
+        <v>25</v>
+      </c>
       <c r="H112">
         <v>135</v>
       </c>
@@ -4594,6 +4927,9 @@
       <c r="E113" s="1">
         <v>2</v>
       </c>
+      <c r="G113">
+        <v>24</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
@@ -4611,6 +4947,9 @@
       <c r="E114" s="1">
         <v>1</v>
       </c>
+      <c r="G114" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="115" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
@@ -4628,6 +4967,9 @@
       <c r="E115" s="1">
         <v>1</v>
       </c>
+      <c r="G115" s="1">
+        <v>24</v>
+      </c>
       <c r="H115" s="1">
         <v>141</v>
       </c>
@@ -4652,6 +4994,9 @@
       <c r="E116" s="1">
         <v>2</v>
       </c>
+      <c r="G116">
+        <v>46</v>
+      </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
@@ -4669,6 +5014,9 @@
       <c r="E117" s="1">
         <v>1</v>
       </c>
+      <c r="G117" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
@@ -4687,6 +5035,9 @@
         <v>2</v>
       </c>
       <c r="F118" s="1"/>
+      <c r="G118" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -4704,6 +5055,9 @@
       <c r="E119" s="1">
         <v>2</v>
       </c>
+      <c r="G119" s="1">
+        <v>46</v>
+      </c>
       <c r="H119">
         <v>40</v>
       </c>
@@ -4727,6 +5081,9 @@
       <c r="E120" s="1">
         <v>1</v>
       </c>
+      <c r="G120" s="1">
+        <v>46</v>
+      </c>
       <c r="H120">
         <v>40</v>
       </c>
@@ -4750,6 +5107,9 @@
       <c r="E121" s="1">
         <v>2</v>
       </c>
+      <c r="G121">
+        <v>67</v>
+      </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -4767,6 +5127,9 @@
       <c r="E122" s="1">
         <v>1</v>
       </c>
+      <c r="G122" s="1">
+        <v>67</v>
+      </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
@@ -4784,6 +5147,9 @@
       <c r="E123" s="1">
         <v>1</v>
       </c>
+      <c r="G123" s="1">
+        <v>67</v>
+      </c>
       <c r="H123">
         <v>53</v>
       </c>
@@ -4807,6 +5173,9 @@
       <c r="E124" s="1">
         <v>2</v>
       </c>
+      <c r="G124" s="1">
+        <v>67</v>
+      </c>
       <c r="H124">
         <v>53</v>
       </c>
@@ -4830,6 +5199,9 @@
       <c r="E125" s="1">
         <v>2</v>
       </c>
+      <c r="G125" s="1">
+        <v>67</v>
+      </c>
       <c r="H125">
         <v>53</v>
       </c>
@@ -4854,6 +5226,9 @@
         <v>1</v>
       </c>
       <c r="F126" s="1"/>
+      <c r="G126">
+        <v>89</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
@@ -4872,6 +5247,9 @@
         <v>1</v>
       </c>
       <c r="F127" s="1"/>
+      <c r="G127" s="1">
+        <v>89</v>
+      </c>
       <c r="H127">
         <v>85</v>
       </c>
@@ -4895,6 +5273,9 @@
       <c r="E128" s="1">
         <v>2</v>
       </c>
+      <c r="G128" s="1">
+        <v>89</v>
+      </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
@@ -4912,6 +5293,9 @@
       <c r="E129" s="1">
         <v>2</v>
       </c>
+      <c r="G129" s="1">
+        <v>89</v>
+      </c>
       <c r="H129" s="1">
         <v>85</v>
       </c>
@@ -4935,6 +5319,9 @@
       <c r="E130" s="1">
         <v>1</v>
       </c>
+      <c r="G130">
+        <v>58</v>
+      </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
@@ -4953,6 +5340,9 @@
         <v>2</v>
       </c>
       <c r="F131" s="1"/>
+      <c r="G131" s="1">
+        <v>58</v>
+      </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
@@ -4970,6 +5360,9 @@
       <c r="E132" s="1">
         <v>1</v>
       </c>
+      <c r="G132" s="1">
+        <v>58</v>
+      </c>
       <c r="H132">
         <v>131</v>
       </c>
@@ -4993,6 +5386,9 @@
       <c r="E133" s="1">
         <v>1</v>
       </c>
+      <c r="G133" s="1">
+        <v>58</v>
+      </c>
       <c r="H133">
         <v>131</v>
       </c>
@@ -5016,6 +5412,9 @@
       <c r="E134" s="1">
         <v>2</v>
       </c>
+      <c r="G134" s="1">
+        <v>58</v>
+      </c>
       <c r="H134">
         <v>131</v>
       </c>
@@ -5039,6 +5438,9 @@
       <c r="E135" s="1">
         <v>1</v>
       </c>
+      <c r="G135">
+        <v>70</v>
+      </c>
     </row>
     <row r="136" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -5056,6 +5458,9 @@
       <c r="E136" s="1">
         <v>1</v>
       </c>
+      <c r="G136" s="1">
+        <v>70</v>
+      </c>
       <c r="L136" s="2"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -5074,6 +5479,9 @@
       <c r="E137" s="1">
         <v>2</v>
       </c>
+      <c r="G137" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="138" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
@@ -5091,6 +5499,9 @@
       <c r="E138" s="1">
         <v>2</v>
       </c>
+      <c r="G138" s="1">
+        <v>70</v>
+      </c>
       <c r="L138" s="2"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
@@ -5109,6 +5520,9 @@
       <c r="E139" s="1">
         <v>1</v>
       </c>
+      <c r="G139">
+        <v>63</v>
+      </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
@@ -5126,6 +5540,9 @@
       <c r="E140" s="1">
         <v>2</v>
       </c>
+      <c r="G140" s="1">
+        <v>63</v>
+      </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
@@ -5143,6 +5560,9 @@
       <c r="E141" s="1">
         <v>2</v>
       </c>
+      <c r="G141">
+        <v>84</v>
+      </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
@@ -5160,6 +5580,9 @@
       <c r="E142" s="1">
         <v>1</v>
       </c>
+      <c r="G142" s="1">
+        <v>84</v>
+      </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
@@ -5177,6 +5600,9 @@
       <c r="E143" s="1">
         <v>1</v>
       </c>
+      <c r="G143">
+        <v>90</v>
+      </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
@@ -5194,6 +5620,9 @@
       <c r="E144" s="1">
         <v>2</v>
       </c>
+      <c r="G144" s="1">
+        <v>90</v>
+      </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
@@ -5211,6 +5640,9 @@
       <c r="E145" s="1">
         <v>1</v>
       </c>
+      <c r="G145" s="1">
+        <v>90</v>
+      </c>
       <c r="H145">
         <v>75</v>
       </c>
@@ -5234,6 +5666,9 @@
       <c r="E146" s="1">
         <v>2</v>
       </c>
+      <c r="G146" s="1">
+        <v>90</v>
+      </c>
       <c r="H146">
         <v>75</v>
       </c>
@@ -5257,6 +5692,9 @@
       <c r="E147" s="1">
         <v>1</v>
       </c>
+      <c r="G147" s="1">
+        <v>90</v>
+      </c>
       <c r="H147">
         <v>75</v>
       </c>
@@ -5280,6 +5718,9 @@
       <c r="E148" s="1">
         <v>2</v>
       </c>
+      <c r="G148" s="1">
+        <v>90</v>
+      </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
@@ -5296,6 +5737,9 @@
       </c>
       <c r="E149" s="1">
         <v>1</v>
+      </c>
+      <c r="G149">
+        <v>62</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5314,6 +5758,9 @@
       <c r="E150" s="1">
         <v>1</v>
       </c>
+      <c r="G150" s="1">
+        <v>62</v>
+      </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
@@ -5331,6 +5778,9 @@
       <c r="E151" s="1">
         <v>2</v>
       </c>
+      <c r="G151" s="1">
+        <v>62</v>
+      </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
@@ -5348,6 +5798,9 @@
       <c r="E152" s="1">
         <v>1</v>
       </c>
+      <c r="G152" s="1">
+        <v>62</v>
+      </c>
       <c r="H152">
         <v>115</v>
       </c>
@@ -5371,6 +5824,9 @@
       <c r="E153" s="1">
         <v>1</v>
       </c>
+      <c r="G153" s="1">
+        <v>62</v>
+      </c>
       <c r="H153" s="1">
         <v>115</v>
       </c>
@@ -5394,6 +5850,9 @@
       <c r="E154" s="1">
         <v>2</v>
       </c>
+      <c r="G154" s="1">
+        <v>62</v>
+      </c>
       <c r="H154" s="1">
         <v>115</v>
       </c>
@@ -5417,6 +5876,9 @@
       <c r="E155" s="1">
         <v>2</v>
       </c>
+      <c r="G155">
+        <v>39</v>
+      </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
@@ -5434,6 +5896,9 @@
       <c r="E156" s="1">
         <v>2</v>
       </c>
+      <c r="G156" s="1">
+        <v>39</v>
+      </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
@@ -5451,6 +5916,9 @@
       <c r="E157" s="1">
         <v>1</v>
       </c>
+      <c r="G157" s="1">
+        <v>39</v>
+      </c>
       <c r="H157">
         <v>75</v>
       </c>
@@ -5471,6 +5939,9 @@
       <c r="E158" s="1">
         <v>1</v>
       </c>
+      <c r="G158" s="1">
+        <v>39</v>
+      </c>
       <c r="H158">
         <v>95</v>
       </c>
@@ -5494,6 +5965,9 @@
       <c r="E159" s="1">
         <v>2</v>
       </c>
+      <c r="G159" s="1">
+        <v>39</v>
+      </c>
       <c r="H159">
         <v>95</v>
       </c>
@@ -5517,6 +5991,9 @@
       <c r="E160" s="1">
         <v>1</v>
       </c>
+      <c r="G160" s="1">
+        <v>39</v>
+      </c>
       <c r="H160">
         <v>172</v>
       </c>
@@ -5537,6 +6014,9 @@
       <c r="E161" s="1">
         <v>1</v>
       </c>
+      <c r="G161" s="1">
+        <v>39</v>
+      </c>
       <c r="H161">
         <v>172</v>
       </c>
@@ -5557,6 +6037,9 @@
       <c r="E162" s="1">
         <v>2</v>
       </c>
+      <c r="G162">
+        <v>47</v>
+      </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
@@ -5574,6 +6057,9 @@
       <c r="E163" s="1">
         <v>1</v>
       </c>
+      <c r="G163" s="1">
+        <v>47</v>
+      </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
@@ -5591,6 +6077,9 @@
       <c r="E164" s="1">
         <v>1</v>
       </c>
+      <c r="G164">
+        <v>87</v>
+      </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
@@ -5608,6 +6097,9 @@
       <c r="E165" s="1">
         <v>2</v>
       </c>
+      <c r="G165" s="1">
+        <v>87</v>
+      </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
@@ -5625,6 +6117,9 @@
       <c r="E166" s="1">
         <v>1</v>
       </c>
+      <c r="G166" s="1">
+        <v>87</v>
+      </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
@@ -5642,6 +6137,9 @@
       <c r="E167" s="1">
         <v>1</v>
       </c>
+      <c r="G167" s="1">
+        <v>87</v>
+      </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
@@ -5659,6 +6157,9 @@
       <c r="E168" s="1">
         <v>2</v>
       </c>
+      <c r="G168" s="1">
+        <v>87</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
@@ -5676,6 +6177,9 @@
       <c r="E169" s="1">
         <v>2</v>
       </c>
+      <c r="G169">
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
@@ -5693,6 +6197,9 @@
       <c r="E170" s="1">
         <v>1</v>
       </c>
+      <c r="G170" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
@@ -5710,6 +6217,9 @@
       <c r="E171" s="1">
         <v>1</v>
       </c>
+      <c r="G171" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
@@ -5727,6 +6237,9 @@
       <c r="E172" s="1">
         <v>1</v>
       </c>
+      <c r="G172">
+        <v>64</v>
+      </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
@@ -5744,6 +6257,9 @@
       <c r="E173" s="1">
         <v>1</v>
       </c>
+      <c r="G173">
+        <v>64</v>
+      </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
@@ -5761,6 +6277,9 @@
       <c r="E174" s="1">
         <v>1</v>
       </c>
+      <c r="G174">
+        <v>64</v>
+      </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
@@ -5778,6 +6297,9 @@
       <c r="E175" s="1">
         <v>2</v>
       </c>
+      <c r="G175">
+        <v>64</v>
+      </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
@@ -5796,6 +6318,9 @@
         <v>1</v>
       </c>
       <c r="F176" s="1"/>
+      <c r="G176">
+        <v>57</v>
+      </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
@@ -5813,6 +6338,9 @@
       <c r="E177" s="1">
         <v>1</v>
       </c>
+      <c r="G177" s="1">
+        <v>57</v>
+      </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
@@ -5830,6 +6358,9 @@
       <c r="E178" s="1">
         <v>2</v>
       </c>
+      <c r="G178" s="1">
+        <v>57</v>
+      </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
@@ -5847,6 +6378,9 @@
       <c r="E179" s="1">
         <v>1</v>
       </c>
+      <c r="G179">
+        <v>21</v>
+      </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
@@ -5864,6 +6398,9 @@
       <c r="E180" s="1">
         <v>1</v>
       </c>
+      <c r="G180" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
@@ -5881,6 +6418,9 @@
       <c r="E181" s="1">
         <v>2</v>
       </c>
+      <c r="G181">
+        <v>53</v>
+      </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
@@ -5898,6 +6438,9 @@
       <c r="E182" s="1">
         <v>1</v>
       </c>
+      <c r="G182" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
@@ -5915,6 +6458,9 @@
       <c r="E183" s="1">
         <v>1</v>
       </c>
+      <c r="G183" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
@@ -5932,6 +6478,9 @@
       <c r="E184" s="1">
         <v>2</v>
       </c>
+      <c r="G184" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
@@ -5949,6 +6498,9 @@
       <c r="E185" s="1">
         <v>1</v>
       </c>
+      <c r="G185" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
@@ -5966,6 +6518,9 @@
       <c r="E186" s="1">
         <v>1</v>
       </c>
+      <c r="G186" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
@@ -5983,6 +6538,9 @@
       <c r="E187" s="1">
         <v>2</v>
       </c>
+      <c r="G187" s="1">
+        <v>53</v>
+      </c>
       <c r="H187">
         <v>31</v>
       </c>
@@ -6006,6 +6564,9 @@
       <c r="E188" s="1">
         <v>2</v>
       </c>
+      <c r="G188">
+        <v>97</v>
+      </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
@@ -6023,6 +6584,9 @@
       <c r="E189" s="1">
         <v>1</v>
       </c>
+      <c r="G189" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
@@ -6040,6 +6604,9 @@
       <c r="E190" s="1">
         <v>2</v>
       </c>
+      <c r="G190" s="1">
+        <v>97</v>
+      </c>
       <c r="H190">
         <v>11</v>
       </c>
@@ -6063,6 +6630,9 @@
       <c r="E191" s="1">
         <v>2</v>
       </c>
+      <c r="G191" s="1">
+        <v>97</v>
+      </c>
       <c r="H191">
         <v>11</v>
       </c>
@@ -6086,6 +6656,9 @@
       <c r="E192" s="1">
         <v>1</v>
       </c>
+      <c r="G192" s="1">
+        <v>97</v>
+      </c>
       <c r="H192">
         <v>145</v>
       </c>
@@ -6106,6 +6679,9 @@
       <c r="E193" s="1">
         <v>2</v>
       </c>
+      <c r="G193">
+        <v>26</v>
+      </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
@@ -6123,6 +6699,9 @@
       <c r="E194" s="1">
         <v>1</v>
       </c>
+      <c r="G194" s="1">
+        <v>26</v>
+      </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
@@ -6140,6 +6719,9 @@
       <c r="E195" s="1">
         <v>1</v>
       </c>
+      <c r="G195" s="1">
+        <v>26</v>
+      </c>
       <c r="H195">
         <v>71</v>
       </c>
@@ -6163,6 +6745,9 @@
       <c r="E196" s="1">
         <v>2</v>
       </c>
+      <c r="G196" s="1">
+        <v>26</v>
+      </c>
       <c r="H196">
         <v>71</v>
       </c>
@@ -6186,6 +6771,9 @@
       <c r="E197" s="1">
         <v>2</v>
       </c>
+      <c r="G197">
+        <v>28</v>
+      </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
@@ -6203,6 +6791,9 @@
       <c r="E198" s="1">
         <v>1</v>
       </c>
+      <c r="G198" s="1">
+        <v>28</v>
+      </c>
       <c r="H198">
         <v>3</v>
       </c>
@@ -6223,6 +6814,9 @@
       <c r="E199" s="1">
         <v>2</v>
       </c>
+      <c r="G199" s="1">
+        <v>28</v>
+      </c>
       <c r="H199">
         <v>3</v>
       </c>
@@ -6246,6 +6840,9 @@
       <c r="E200" s="1">
         <v>2</v>
       </c>
+      <c r="G200" s="1">
+        <v>28</v>
+      </c>
       <c r="H200">
         <v>3</v>
       </c>
@@ -6269,6 +6866,9 @@
       <c r="E201" s="1">
         <v>1</v>
       </c>
+      <c r="G201" s="1">
+        <v>28</v>
+      </c>
       <c r="H201">
         <v>70</v>
       </c>
@@ -6289,6 +6889,9 @@
       <c r="E202" s="1">
         <v>2</v>
       </c>
+      <c r="G202">
+        <v>66</v>
+      </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
@@ -6306,6 +6909,9 @@
       <c r="E203" s="1">
         <v>2</v>
       </c>
+      <c r="G203" s="1">
+        <v>66</v>
+      </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
@@ -6323,6 +6929,9 @@
       <c r="E204" s="1">
         <v>1</v>
       </c>
+      <c r="G204" s="1">
+        <v>66</v>
+      </c>
       <c r="H204">
         <v>43</v>
       </c>
@@ -6343,6 +6952,9 @@
       <c r="E205" s="1">
         <v>1</v>
       </c>
+      <c r="G205" s="1">
+        <v>43</v>
+      </c>
       <c r="H205">
         <v>26</v>
       </c>
@@ -6366,6 +6978,9 @@
       <c r="E206" s="1">
         <v>2</v>
       </c>
+      <c r="G206" s="1">
+        <v>43</v>
+      </c>
       <c r="H206">
         <v>43</v>
       </c>
@@ -6387,7 +7002,10 @@
         <v>40</v>
       </c>
       <c r="E207" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G207">
+        <v>4</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6406,8 +7024,11 @@
       <c r="E208" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G208" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>212</v>
       </c>
@@ -6421,10 +7042,13 @@
         <v>40</v>
       </c>
       <c r="E209" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G209" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>218</v>
       </c>
@@ -6440,8 +7064,11 @@
       <c r="E210" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G210">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>231</v>
       </c>
@@ -6455,10 +7082,13 @@
         <v>40</v>
       </c>
       <c r="E211" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G211" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>247</v>
       </c>
@@ -6472,10 +7102,13 @@
         <v>40</v>
       </c>
       <c r="E212" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G212" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>254</v>
       </c>
@@ -6491,8 +7124,11 @@
       <c r="E213" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G213" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>214</v>
       </c>
@@ -6508,8 +7144,11 @@
       <c r="E214" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G214">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>221</v>
       </c>
@@ -6525,8 +7164,11 @@
       <c r="E215" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G215" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>230</v>
       </c>
@@ -6542,8 +7184,11 @@
       <c r="E216" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G216" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>245</v>
       </c>
@@ -6559,8 +7204,11 @@
       <c r="E217" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G217" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>206</v>
       </c>
@@ -6576,8 +7224,11 @@
       <c r="E218" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G218">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>248</v>
       </c>
@@ -6593,8 +7244,11 @@
       <c r="E219" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G219" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>253</v>
       </c>
@@ -6610,8 +7264,11 @@
       <c r="E220" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G220" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>207</v>
       </c>
@@ -6627,8 +7284,11 @@
       <c r="E221" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G221">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>234</v>
       </c>
@@ -6644,8 +7304,11 @@
       <c r="E222" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G222" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>238</v>
       </c>
@@ -6661,8 +7324,11 @@
       <c r="E223" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G223" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>240</v>
       </c>
@@ -6678,8 +7344,11 @@
       <c r="E224" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G224" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>255</v>
       </c>
@@ -6695,8 +7364,11 @@
       <c r="E225" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G225" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>211</v>
       </c>
@@ -6712,8 +7384,11 @@
       <c r="E226" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>228</v>
       </c>
@@ -6729,8 +7404,11 @@
       <c r="E227" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G227" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>235</v>
       </c>
@@ -6746,8 +7424,11 @@
       <c r="E228" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G228" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>236</v>
       </c>
@@ -6763,8 +7444,11 @@
       <c r="E229" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G229" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -6780,8 +7464,11 @@
       <c r="E230" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G230">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>241</v>
       </c>
@@ -6797,8 +7484,11 @@
       <c r="E231" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G231" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>251</v>
       </c>
@@ -6814,8 +7504,11 @@
       <c r="E232" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G232" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>252</v>
       </c>
@@ -6831,8 +7524,11 @@
       <c r="E233" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G233" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>258</v>
       </c>
@@ -6848,8 +7544,11 @@
       <c r="E234" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G234" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>209</v>
       </c>
@@ -6865,8 +7564,11 @@
       <c r="E235" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G235">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>223</v>
       </c>
@@ -6882,8 +7584,11 @@
       <c r="E236" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G236" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>225</v>
       </c>
@@ -6899,8 +7604,11 @@
       <c r="E237" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G237" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>232</v>
       </c>
@@ -6916,8 +7624,11 @@
       <c r="E238" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G238" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -6933,8 +7644,11 @@
       <c r="E239" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G239">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -6950,8 +7664,11 @@
       <c r="E240" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G240" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>243</v>
       </c>
@@ -6967,8 +7684,11 @@
       <c r="E241" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G241" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>219</v>
       </c>
@@ -6984,8 +7704,11 @@
       <c r="E242" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G242">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>222</v>
       </c>
@@ -7001,8 +7724,11 @@
       <c r="E243" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G243" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>244</v>
       </c>
@@ -7018,8 +7744,11 @@
       <c r="E244" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G244" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>256</v>
       </c>
@@ -7035,8 +7764,11 @@
       <c r="E245" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G245" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>257</v>
       </c>
@@ -7052,8 +7784,11 @@
       <c r="E246" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G246" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>213</v>
       </c>
@@ -7069,8 +7804,11 @@
       <c r="E247" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G247">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>215</v>
       </c>
@@ -7086,8 +7824,11 @@
       <c r="E248" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G248" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>216</v>
       </c>
@@ -7103,8 +7844,11 @@
       <c r="E249" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G249" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>220</v>
       </c>
@@ -7120,8 +7864,11 @@
       <c r="E250" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G250" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>226</v>
       </c>
@@ -7137,8 +7884,11 @@
       <c r="E251" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G251" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>227</v>
       </c>
@@ -7154,8 +7904,11 @@
       <c r="E252" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G252">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>233</v>
       </c>
@@ -7169,10 +7922,13 @@
         <v>48</v>
       </c>
       <c r="E253" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G253" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>242</v>
       </c>
@@ -7186,10 +7942,13 @@
         <v>48</v>
       </c>
       <c r="E254" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G254" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>250</v>
       </c>
@@ -7203,10 +7962,13 @@
         <v>48</v>
       </c>
       <c r="E255" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G255" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>259</v>
       </c>
@@ -7222,8 +7984,11 @@
       <c r="E256" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G256" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>217</v>
       </c>
@@ -7239,8 +8004,11 @@
       <c r="E257" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G257">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>224</v>
       </c>
@@ -7256,8 +8024,11 @@
       <c r="E258" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G258" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>246</v>
       </c>
@@ -7273,8 +8044,11 @@
       <c r="E259" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G259" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>249</v>
       </c>
@@ -7289,6 +8063,9 @@
       </c>
       <c r="E260" s="1">
         <v>2</v>
+      </c>
+      <c r="G260" s="1">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>